<commit_message>
Updated VSL paper and JMP
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grady\Documents\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E913A40-AB28-4CAB-BC7B-250FFAA36737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407FDEB4-C1FD-4B9D-90C7-09628B673E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
   </bookViews>
@@ -100,13 +100,13 @@
     <t>with Supreet Kaur</t>
   </si>
   <si>
-    <t xml:space="preserve">Economists often study preferences for non-market goods such as health. This paper introduces a new method to estimate demand for such amenities and applies it to measure the value of a statistical life (VSL) in Kenya. My approach is to update beliefs about the efficacy of a product that reduces mortality risk (a helmet) and elicit product choice. This generates instruments allowing one to use subjective beliefs to estimate demand, rather than assuming rational expectations. This procedure does not require beliefs to be reported error-free but does require classical mismeasurement. I validate this assumption using insights from the local average treatment effects literature. The method estimates a VSL of $224, near the left tail of estimates. Existing methods for estimating VSL produce skewed results, driven by severe violations of rational expectations. These findings rationalize low demand for health products and suggest that billions of dollars of development aid is misallocated. </t>
-  </si>
-  <si>
     <t>Latex</t>
   </si>
   <si>
-    <t>I report the results of two randomized controlled trials in Kenya demonstrating that retail firms under-adopt new products because they are risk averse and face uncertain demand. The experiments study the market for motorcycle helmets, which many shops believe are profitable, yet few adopt. One experiment $(N=350)$ offers shops a contract that induces a mean-preserving contraction of profits. This increases stocking from 20\% to 30\%, indicating that risk aversion constrains adoption. The second experiment $(N=929)$ allows treated firms to return unsold stock, a common high-income policy. Shops offered returns are more than twice as likely (10 p.p.) to try selling helmets, yet only 5 shops make returns. Effects are persistent. Treated firms are 7 p.p. (70\%) more likely to stock after the returns window ends and most stay in the market. Belief data indicates that returns crowd in shops with diffuse priors about demand whose uncertainty is resolved by experience, consistent with learning by risk averse agents. A second experimental arm supports this interpretation by reducing future supply chain uncertainty, making learning more valuable. This doubles adoption if shops cannot return stock but has no effect if they can. This matches theoretical predictions since returns eliminate losses, inducing any firm uncertain about the profitability of helmets to stock. These results suggest that products may diffuse inefficiently in low and middle-income economies because small retailers pay a high utility cost to experiment with new goods. The findings also call into question the common practice of modeling small enterprises as risk neutral.</t>
+    <t xml:space="preserve">Economists often study non-market goods such as health and air quality. This paper introduces a new method to estimate demand for such amenities and applies it to measure the value of a statistical life (VSL) in Kenya. My approach is to update beliefs about the life-saving efficacy of a product (a motorcycle helmet) and elicit product choice. This generates instruments allowing one to use subjective beliefs to estimate demand, rather than assuming rational expectations. This method does not require beliefs to be reported error-free but does require classical mismeasurement. I validate this assumption using features of the experimental design. The estimated VSL is \$224, near the left tail of Kenyan estimates. Standard methods for estimating VSL produce skewed results, driven by severe violations of rational expectations. These findings help explain low observed demand for many health products and suggest that directing more development aid towards consumption may increase welfare. </t>
+  </si>
+  <si>
+    <t>Economists typically assume that firms are risk neutral. Yet many enterprises, especially in low and middle-income economies, are small and owner-operated, making household consumption sensitive to business risk. This may cause the risk preferences of firm owners to affect firm decisions. This paper demonstrates that small retailers in Kenya are risk averse, leading them to under-adopt a new product because they face uncertain demand. I develop a model in which risk averse firms learn about demand through stocking decisions, then test its predictions using two field experiments. The first establishes that risk aversion affects the stocking decisions of enterprises. I construct a new test for risk aversion by offering treated firms an insurance contract that lowers expected profits from a new product and reduces the risk of losses, leading to a 50\% increase in adoption which implies a rejection of risk neutrality. The second experiment shows that \textit{temporarily} reducing inventory risk leads firms to \textit{permanently} stock a profitable new product because they overcome demand uncertainty through learning. These results suggest a departure from perfect competition, since risk averse firms are not competed out of the market. I document information externalities consistent with this prediction: enterprises that are nearby randomly induced entrants stock the new product at a higher rate. These results suggest that risk aversion can impede product diffusion and firm growth, challenging the common assumption that small firms are risk neutral.</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
@@ -543,15 +543,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
@@ -605,7 +608,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="348" x14ac:dyDescent="0.35">
@@ -661,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added NBER IMR draft to website
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grady\Documents\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2058D250-1653-473C-89A8-CFDD28387892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43EC92F-497B-4F59-8846-C973A8C00121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Title</t>
   </si>
@@ -67,15 +67,9 @@
     <t>https://github.com/gkilleen33/gkilleen33.github.io/blob/master/papers/working/Killeen-JMP.pdf</t>
   </si>
   <si>
-    <t>Unconditional Cash Transfers and Child Mortality: Experimental Evidence from Kenya</t>
-  </si>
-  <si>
     <t>with Michael Walker, Nick Shankar, Edward Miguel and Dennis Egger</t>
   </si>
   <si>
-    <t>We estimate the intergenerational health impacts of large-scale unconditional cash transfers. One-time transfers of USD 1000 were provided to over 10,500 poor households across 653 randomized villages in Kenya. We collected regional census data on over 100,000 births, including on mortality and cause of death, and detailed data on household health behaviors. In the study's main finding, the cash transfer treatment leads to 55% fewer infant deaths before age one and 49% fewer child deaths before age five. Data on the location of health facilities, as well as the cause of death and transfer timing relative to birth, indicate that unconditional cash transfers and access to delivery services are complements in generating mortality reductions: the largest gains are estimated among households living close to health facilities who receive the transfer around the time of the birth, and treatment leads to a large overall increase in hospital deliveries. Infant and child mortality then largely revert to pre-program levels after cash transfers end. Despite not being the main aim of the original program, we show that unconditional cash transfers in this setting may be a cost-effective way to reduce infant and child deaths.</t>
-  </si>
-  <si>
     <t>Using satellites and phones to evaluate and promote agricultural technology adoption: Evidence from smallholder farms in India</t>
   </si>
   <si>
@@ -91,9 +85,6 @@
     <t>Free-Riding and New Product Adoption: Evidence from Burundi</t>
   </si>
   <si>
-    <t>with Luisa Cefala, Rédempteur Ntawiratsa and Nicholas Swanson</t>
-  </si>
-  <si>
     <t>Multiple Missing Markets and Allocative Efficiency</t>
   </si>
   <si>
@@ -107,13 +98,50 @@
   </si>
   <si>
     <t>Economists typically view firms as risk neutral. Yet many enterprises, especially in low and middle-income economies, are small and owner-operated, making household consumption sensitive to business risk. As a result, owners' risk preferences may influence firm decisions. This paper demonstrates that small retailers in Kenya are risk averse, leading them to under-adopt a new product when they face uncertain demand. I model risk averse firms who learn about demand through stocking decisions, then test the model's predictions using two field experiments. The first establishes that risk aversion affects the stocking decisions of enterprises. I test for risk aversion by offering treated firms an insurance contract that lowers expected profits from a new product and reduces the risk of losses, leading to a 50\% increase in adoption. This rejects risk neutrality. The second experiment shows that \textit{temporarily} reducing inventory risk leads firms to \textit{permanently} stock a profitable new product because they overcome demand uncertainty through learning. These results show that risk aversion can impede product diffusion, challenging the common assumption that small firms are risk neutral.</t>
+  </si>
+  <si>
+    <t>Can Cash Transfers Save Lives? Evidence from a Large-Scale Experiment in Kenya</t>
+  </si>
+  <si>
+    <t>We estimate the impacts of large-scale unconditional cash transfers on child survival. One-time transfers of USD 1000 were provided to over 10,500 poor households across 653 randomized villages in Kenya. We collected census data on over 100,000 births, including on mortality and cause of death, and detailed data on household health behaviors. Unconditional cash transfers (accounting for spillovers) lead to 48\% fewer infant deaths before age one and 45\% fewer child deaths before age five. Detailed data on cause of death, transfer timing relative to birth, and the location of health facilities indicate that unconditional cash transfers and access to delivery care are complements in generating mortality reductions: the largest gains are estimated in neonatal and maternal causes of death largely preventable by appropriate obstetric care and among households living close to physician-staffed facilities and those who receive the transfer around the time of birth, and treatment leads to a large increase in hospital deliveries (by 45\%). The infant and child mortality declines are concentrated among poorer households with below median assets or predicted consumption. The transfers also result in a substantial decline of 51\% in female labor supply in the three months before and the three months after a birth, and improved child nutrition. Infant and child mortality largely revert to pre-program levels after cash transfers end. Despite not being the main aim of the original program, we show that unconditional cash transfers in this setting may be a cost-effective way to reduce infant and child deaths.</t>
+  </si>
+  <si>
+    <t>https://github.com/gkilleen33/gkilleen33.github.io/blob/master/papers/working/GE-IMR.pdf</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Data collection in process </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with Luisa Cefala, Rédempteur Ntawiratsa and Nicholas Swanson</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">In low and middle-income (LMIC) countries, businesses often use technologies inside the frontier, innovate less, and slowly adopt new products and technologies (Cirera et al. 2022). The reasons for these facts are not well understood, particularly for small and microenterprises (e.g. Atkin et al. 2017). 
+We investigate whether a lack of institutions to protect the value of intellectual property contributes to these facts. High-income economies tend to have strong patent systems to promote discoveries, and regulators permit exclusive dealing in retail environments due to similar forces. But LMIC firms are often informal and undifferentiated, meaning neighbours are likely to adopt discoveries of their competitors without compensation. 
+This project focuses on this problem in the case of retail firms’ decision to adopt a new product-- a setting where firms face risk ex-ante because they do not know if demand will exist, but, ex-post, competitors can learn if demand is high by observing the first mover. We examine whether offering retailers exclusive access to supply of a new product promotes adoption. Our study also tests whether firms are colluding so that if there is a null result we can understand if it is due to collusion, a possible upside to the finding that some markets in LMICs are uncompetitive (Bergquist and Dinerstein 2020). </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +153,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -496,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F856E6-0DAE-4AB0-8DFD-4ED5A926F3C8}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -523,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
@@ -534,7 +570,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -548,7 +584,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -559,19 +595,26 @@
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{C80A6612-84C5-4740-9FA9-F56BA622C6F1}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{11D16F1B-AD82-48FA-9833-445D3F3963E4}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{DFD0FFEB-B84A-4674-A8C7-B7EC4F6A8DC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -608,21 +651,21 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -638,7 +681,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,23 +707,26 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated JMP draft and added long run GE
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grady\Documents\website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grady\Documents\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123DEB12-8AA3-44D4-B41B-96377D435E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02E7FED-48DD-4084-B8F0-F7952D038DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Working Papers" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Title</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">Economists often study non-market goods such as health and air quality. This paper introduces a new method to estimate demand for such amenities and applies it to measure the value of a statistical life (VSL) in Kenya. My approach is to update beliefs about the life-saving efficacy of a product (a motorcycle helmet) and elicit product choice. This generates instruments allowing one to use subjective beliefs to estimate demand, rather than assuming rational expectations. This method does not require beliefs to be reported error-free but does require classical mismeasurement. I validate this assumption using features of the experimental design. The estimated VSL is \$224, near the left tail of Kenyan estimates. Standard methods for estimating VSL produce skewed results, driven by severe violations of rational expectations. These findings help explain low observed demand for many health products and suggest that directing more development aid towards consumption may increase welfare. </t>
-  </si>
-  <si>
-    <t>Economists typically view firms as risk neutral. Yet many enterprises, especially in low and middle-income economies, are small and owner-operated, making household consumption sensitive to business risk. As a result, owners' risk preferences may influence firm decisions. This paper demonstrates that small retailers in Kenya are risk averse, leading them to under-adopt a new product when they face uncertain demand. I model risk averse firms who learn about demand through stocking decisions, then test the model's predictions using two field experiments. The first establishes that risk aversion affects the stocking decisions of enterprises. I test for risk aversion by offering treated firms an insurance contract that lowers expected profits from a new product and reduces the risk of losses, leading to a 50\% increase in adoption. This rejects risk neutrality. The second experiment shows that \textit{temporarily} reducing inventory risk leads firms to \textit{permanently} stock a profitable new product because they overcome demand uncertainty through learning. These results show that risk aversion can impede product diffusion, challenging the common assumption that small firms are risk neutral.</t>
   </si>
   <si>
     <t>Can Cash Transfers Save Lives? Evidence from a Large-Scale Experiment in Kenya</t>
@@ -135,6 +132,18 @@
   </si>
   <si>
     <t>with Shawn Cole, Aparna Krishna and Tomoko Harigaya. Journal of Development Economics.</t>
+  </si>
+  <si>
+    <t>Economists typically view firms as risk neutral. Yet many enterprises, especially in low and middle-income economies, are small and owner-operated, making household consumption sensitive to business risk. As a result, owners' risk preferences may influence firm decisions. This paper demonstrates that small retailers in Kenya are risk averse, leading them to under-adopt a new product when they face uncertain demand. I model risk averse firms who learn about demand through stocking decisions, then test the model's predictions using two field experiments. The first establishes that risk aversion affects the stocking decisions of enterprises. I test for risk aversion by offering treated firms an insurance contract that lowers expected profits from a new product while reducing the risk of losses. This leads to a 50\% increase in adoption, rejecting risk neutrality. The second experiment shows that \textit{temporarily} reducing inventory risk leads firms to \textit{permanently} stock a profitable new product because they overcome demand uncertainty through learning. These results show that risk aversion in firms can impede product diffusion, potentially limiting growth.</t>
+  </si>
+  <si>
+    <t>The Long-run Effects of Unconditional Cash Transfers: Evidence from the Kenya General Equilibrium Study</t>
+  </si>
+  <si>
+    <t>with Dennis Egger, Edward Miguel and Michael Walker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recent studies document positive short-run effects of unconditional cash transfers (UCTs) on cash recipients and spillover effects on non-recipients. But modest sample sizes and challenges with tracking households over time have limited research on the long-run effects of UCTs. We study the long-run effects of the Kenya General Equilibrium Study (KGES) on recipient households and the local economy using census and survey data collected up to ten years post-transfers. An “endline 2” completed 4-7 years after the transfers collected census data from each household and enterprise in the study area, and a representative survey of more than 10,000 households and firms obtained more detailed consumption and production measures for a subset, including from those that migrated out of the study area. We collected this same information in an “endline 3” completed 7-10 years after the experimental start. Preliminary results from endline 2 show persistent consumption gains among recipients and expansion of non-farm enterprise revenue. Ongoing analysis examines whether these effects persisted to endline 3 and aims to estimate long-run transfer multipliers. </t>
   </si>
 </sst>
 </file>
@@ -533,19 +542,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -570,7 +579,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
@@ -579,9 +588,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -593,18 +602,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -624,20 +633,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4634DBF9-2A4B-4BD6-9503-80AC50EBF305}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,12 +663,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -678,22 +687,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72C59CF-0C37-4915-9D99-95832D380190}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,23 +719,34 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Typo fix in URL
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grady\Documents\website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grady\Documents\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E01708-3532-418D-A4F1-43CD61A97174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F064D5-74E9-4E14-A6A5-71F12CBE9FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Working Papers" sheetId="1" r:id="rId1"/>
@@ -131,10 +131,10 @@
     <t>https://gkilleen33.github.io/papers/working/Killeen-VSL.pdf</t>
   </si>
   <si>
-    <t>https://ggkilleen33.github.io/papers/working/GE-IMR.pdf</t>
-  </si>
-  <si>
     <t>https://gkilleen33.github.io/papers/working/Killeen-JMP.pdf</t>
+  </si>
+  <si>
+    <t>https://gkilleen33.github.io/papers/working/GE-IMR.pdf</t>
   </si>
 </sst>
 </file>
@@ -532,20 +532,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F856E6-0DAE-4AB0-8DFD-4ED5A926F3C8}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,7 +562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -573,13 +573,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -604,7 +604,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -628,16 +628,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +654,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -684,16 +684,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,7 +710,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -721,7 +721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Updated abstract for JMP
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grady\Documents\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605B3B8F-0DF0-49DF-81D3-448B29BEE264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046269EE-6A0B-413F-AC63-9B2EDD950710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>Latex</t>
   </si>
   <si>
-    <t>Economists typically view firms as risk neutral. Yet many enterprises, especially in low and middle-income economies, are small and owner-operated, making household consumption sensitive to business risk. As a result, owners' risk preferences may influence firm decisions. This paper demonstrates that small retailers in Kenya are risk averse, leading them to under-adopt a new product when they face uncertain demand. I model risk averse firms who learn about demand through stocking decisions, then test the model's predictions using two field experiments. The first establishes that risk aversion affects the stocking decisions of enterprises. I test for risk aversion by offering treated firms an insurance contract that lowers expected profits from a new product and reduces the risk of losses, leading to a 50\% increase in adoption. This rejects risk neutrality. The second experiment shows that \textit{temporarily} reducing inventory risk leads firms to \textit{permanently} stock a profitable new product because they overcome demand uncertainty through learning. These results show that risk aversion can impede product diffusion, challenging the common assumption that small firms are risk neutral.</t>
-  </si>
-  <si>
     <t>Can Cash Transfers Save Lives? Evidence from a Large-Scale Experiment in Kenya</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>https://gkilleen33.github.io/papers/working/GE-IMR.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firms in low and middle-income economies often grow slowly, with limited entrepreneurship and innovation. This paper examines whether firm risk aversion prevents risk taking necessary to grow. Because many firms in developing countries are owner-operated, uncertain investments may directly threaten owners’ consumption. I develop a model of small firm learning which shows that risk aversion can impede product adoption by preventing experimentation with new goods. I test the model using two field experiments in Kenya. Offering shops stock of a new product with insurance that reduces potential losses but lowers expected profits raises stocking by 50\%, rejecting risk neutrality. Inducing firms to try stocking the product with a temporary return policy leads to a 70\% increase in stocking after the intervention ends. Firms experiment more when the continuation value of learning increases. The return policy induces risk averse firms uncertain about demand to stock, who overcome uncertainty by learning. These results show that risk aversion can undermine firm learning, preventing enterprises from stocking profitable goods. </t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F856E6-0DAE-4AB0-8DFD-4ED5A926F3C8}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,7 +562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -570,10 +570,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -581,13 +581,13 @@
     </row>
     <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -595,16 +595,16 @@
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -659,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -715,10 +715,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated JMP title and abstract
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grady\Documents\website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grady\Documents\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046269EE-6A0B-413F-AC63-9B2EDD950710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7A6B0D-6AF3-41FA-9187-3EC7EE8D6968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Working Papers" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>&lt;b&gt;Job Market Paper&lt;/b&gt;</t>
   </si>
   <si>
-    <t>Risk Aversion and Demand Uncertainty Among Small Firms: Evidence From New Product Adoption</t>
-  </si>
-  <si>
     <t>with Michael Walker, Nick Shankar, Edward Miguel and Dennis Egger</t>
   </si>
   <si>
@@ -134,7 +131,10 @@
     <t>https://gkilleen33.github.io/papers/working/GE-IMR.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">Firms in low and middle-income economies often grow slowly, with limited entrepreneurship and innovation. This paper examines whether firm risk aversion prevents risk taking necessary to grow. Because many firms in developing countries are owner-operated, uncertain investments may directly threaten owners’ consumption. I develop a model of small firm learning which shows that risk aversion can impede product adoption by preventing experimentation with new goods. I test the model using two field experiments in Kenya. Offering shops stock of a new product with insurance that reduces potential losses but lowers expected profits raises stocking by 50\%, rejecting risk neutrality. Inducing firms to try stocking the product with a temporary return policy leads to a 70\% increase in stocking after the intervention ends. Firms experiment more when the continuation value of learning increases. The return policy induces risk averse firms uncertain about demand to stock, who overcome uncertainty by learning. These results show that risk aversion can undermine firm learning, preventing enterprises from stocking profitable goods. </t>
+    <t>Many enterprises in low and middle-income countries (LMICs) are owner-operated, so uncertain investments directly impact household consumption. This paper asks whether this link results in risk aversion that prevents firms from making uncertain investments needed to grow. I develop a model of small firm learning which shows that risk aversion can impede product adoption by preventing experimentation with new goods. I test the model using two field experiments in Kenya. The first directly tests whether risk aversion affects product stocking. Firms were offered new product inventory with an insurance contract that would be strictly dominated under risk neutrality. This increased adoption by 50\%, rejecting firm risk neutrality. The second experiment examines longer-run effects. Temporarily inducing firms to try selling a new product with a supplier returns policy led to a 70\% increase in stocking \textit{after} the intervention ended. The policy encouraged uncertain but optimistic firms to experiment, and they resolved uncertainty through learning. I validate the importance of learning by showing that firms were more willing to stock when the continuation value of learning increased, and when firms received information about demand. These results show that risk aversion can prevent small firms from making uncertain but high expected return investments, creating a barrier to growth that is not captured by standard models that assume risk neutral firms.</t>
+  </si>
+  <si>
+    <t>Risk Aversion and Barriers to Firm Growth: Experimental Evidence from Small Retailers</t>
   </si>
 </sst>
 </file>
@@ -533,19 +533,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,52 +559,52 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -628,16 +628,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -651,21 +651,21 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -684,16 +684,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.90625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,26 +707,26 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missing KGES long run abstract
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grady\Documents\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1153F2E7-7A12-49EE-B971-456957B4EE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64DBCC8-D129-48B4-BD08-00C88A17F52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Working Papers" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Title</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>Firms in low and middle-income economies often grow slowly. This paper examines whether firm risk aversion prevents risk taking necessary to grow. While economists tend to model firms as risk neutral, I posit that this assumption is unlikely to hold for the modal developing country firm, which is owner-operated, so that uncertain investments may directly threaten owners’ consumption. I develop a model that shows how risk aversion can reduce firms’ willingness to experiment with new technologies, impeding investment and growth. I test the model’s predictions within the context of retail firms’ decision to adopt and sell a new consumer product using two field experiments with over 1,200 Kenyan firms. First, offering firms an insurance contract that creates a mean-preserving contraction of profits increases new product adoption by 50\%. Effects are concentrated among firms whose owners exhibit higher levels of risk aversion. Second, temporarily inducing firms to try selling a new product with a supplier returns policy leads to a 70\% increase in stock purchases after the intervention ends. Third, consistent with bandit models of learning, experimentally increasing the continuation value of learning increases adoption by 80\%. These persistent effects arise through a reduction in the variance of beliefs, rather than through changes in mean beliefs. These results show that a feature inherent to developing country environments -- small firms in the presence of missing financial markets -- itself creates a barrier to firm innovation and growth.</t>
+  </si>
+  <si>
+    <t>The Long-run Effects of Unconditional Cash Transfers: Evidence from the Kenya General Equilibrium Study</t>
+  </si>
+  <si>
+    <t>with Dennis Egger, Edward Miguel and Michael Walker</t>
+  </si>
+  <si>
+    <t>Recent studies document positive short-run effects of unconditional cash transfers (UCTs) on cash recipients and spillover effects on non-recipients. But modest sample sizes and challenges with tracking households over time have limited research on the long-run effects of UCTs. We study the long-run effects of the Kenya General Equilibrium Study (KGES) on recipient households and the local economy using census and survey data collected up to ten years post-transfers. An “endline 2” completed 4-7 years after the transfers collected census data from each household and enterprise in the study area, and a representative survey of more than 10,000 households and firms obtained more detailed consumption and production measures for a subset, including from those that migrated out of the study area. We collected this same information in an “endline 3” completed 7-10 years after the experimental start. Preliminary results from endline 2 show persistent consumption gains among recipients and expansion of non-farm enterprise revenue. Ongoing analysis examines whether these effects persisted to endline 3 and aims to estimate long-run transfer multipliers.</t>
   </si>
 </sst>
 </file>
@@ -532,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F856E6-0DAE-4AB0-8DFD-4ED5A926F3C8}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -678,10 +687,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72C59CF-0C37-4915-9D99-95832D380190}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,6 +738,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated VSL paper draft
</commit_message>
<xml_diff>
--- a/papers.xlsx
+++ b/papers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grady\Documents\personal-website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grady/Documents/personal-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64DBCC8-D129-48B4-BD08-00C88A17F52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E921F20-E099-A544-BF24-9BECB5A1EABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
+    <workbookView xWindow="-46860" yWindow="-6440" windowWidth="31600" windowHeight="20280" xr2:uid="{97D96D2E-9D3E-43F7-890C-EE13786D0DA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Working Papers" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>https://gkilleen33.github.io/papers/working/Killeen-JMP.pdf</t>
   </si>
   <si>
-    <t>This paper introduces a new method for estimating demand for non-market goods and applies it to the value of a statistical life (VSL) in Kenya. The approach updates beliefs about the life-saving efficacy of a product (helmets) and elicits product choice. This allows demand to be estimated from subjective beliefs rather than assuming rational expectations. The resulting VSL estimate is \$224, near the lower end of Kenyan estimates. Standard methods produce skewed results, driven by violations of rational expectations. The findings help explain weak demand for preventive health and suggest that redirecting some development aid toward consumption could raise welfare.</t>
-  </si>
-  <si>
     <t>https://gkilleen33.github.io/papers/working/GE-IMR.pdf</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>Recent studies document positive short-run effects of unconditional cash transfers (UCTs) on cash recipients and spillover effects on non-recipients. But modest sample sizes and challenges with tracking households over time have limited research on the long-run effects of UCTs. We study the long-run effects of the Kenya General Equilibrium Study (KGES) on recipient households and the local economy using census and survey data collected up to ten years post-transfers. An “endline 2” completed 4-7 years after the transfers collected census data from each household and enterprise in the study area, and a representative survey of more than 10,000 households and firms obtained more detailed consumption and production measures for a subset, including from those that migrated out of the study area. We collected this same information in an “endline 3” completed 7-10 years after the experimental start. Preliminary results from endline 2 show persistent consumption gains among recipients and expansion of non-farm enterprise revenue. Ongoing analysis examines whether these effects persisted to endline 3 and aims to estimate long-run transfer multipliers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Economists often study non-market goods such as health and air quality. This paper introduces a new method to estimate demand for such amenities and applies it to measure the value of a statistical life (VSL) in Kenya. My approach is to update beliefs about the life-saving efficacy of a product (a motorcycle helmet) and elicit product choice. This generates instruments allowing one to use subjective beliefs to estimate demand, rather than assuming rational expectations. This method does not require beliefs to be reported error-free but does require classical mismeasurement. I validate this assumption using features of the experimental design. The estimated VSL is \$224, near the left tail of Kenyan estimates. Standard methods for estimating VSL produce skewed results, driven by severe violations of rational expectations. These findings help explain low observed demand for many health products and suggest that directing more development aid towards consumption may increase welfare. </t>
   </si>
 </sst>
 </file>
@@ -541,20 +541,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F856E6-0DAE-4AB0-8DFD-4ED5A926F3C8}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="38.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,15 +570,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>20</v>
@@ -588,12 +587,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="350" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -602,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -613,7 +612,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -637,16 +636,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="38.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="335" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -689,20 +687,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72C59CF-0C37-4915-9D99-95832D380190}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="38.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -730,7 +727,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -738,15 +735,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>